<commit_message>
Update model 7/1/2025 6:50 PM UTC
</commit_message>
<xml_diff>
--- a/old_models/accuracies/max_r_model_accuracies.xlsx
+++ b/old_models/accuracies/max_r_model_accuracies.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9609120521172638</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="C2" t="n">
-        <v>0.749185667752443</v>
+        <v>0.7694805194805194</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9609120521172638</v>
+        <v>0.9675324675324676</v>
       </c>
       <c r="C3" t="n">
-        <v>0.758957654723127</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9739413680781759</v>
+        <v>0.9707792207792207</v>
       </c>
       <c r="C4" t="n">
-        <v>0.739413680781759</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9674267100977199</v>
+        <v>0.974025974025974</v>
       </c>
       <c r="C5" t="n">
-        <v>0.758957654723127</v>
+        <v>0.762987012987013</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9641693811074918</v>
+        <v>0.9675324675324676</v>
       </c>
       <c r="C6" t="n">
-        <v>0.739413680781759</v>
+        <v>0.7305194805194806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update model 7/1/2024 10:22 PM 90/10 old
</commit_message>
<xml_diff>
--- a/old_models/accuracies/max_r_model_accuracies.xlsx
+++ b/old_models/accuracies/max_r_model_accuracies.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9642857142857143</v>
+        <v>0.9579288025889967</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7694805194805194</v>
+        <v>0.8058252427184466</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9675324675324676</v>
+        <v>0.9676375404530745</v>
       </c>
       <c r="C3" t="n">
-        <v>0.75</v>
+        <v>0.8381877022653722</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9707792207792207</v>
+        <v>0.9741100323624595</v>
       </c>
       <c r="C4" t="n">
-        <v>0.75</v>
+        <v>0.7702265372168284</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.974025974025974</v>
+        <v>0.9676375404530745</v>
       </c>
       <c r="C5" t="n">
-        <v>0.762987012987013</v>
+        <v>0.8284789644012945</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9675324675324676</v>
+        <v>0.9644012944983819</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7305194805194806</v>
+        <v>0.8058252427184466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update models 7/2/2025 7:22 PM 3093
</commit_message>
<xml_diff>
--- a/old_models/accuracies/max_r_model_accuracies.xlsx
+++ b/old_models/accuracies/max_r_model_accuracies.xlsx
@@ -453,66 +453,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RandomForest Max R</t>
+          <t>RandomForest Multi-Max R</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9579288025889967</v>
+        <v>0.9548387096774194</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8058252427184466</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>XGBoost Max R</t>
+          <t>XGBoost Multi-Max R</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9676375404530745</v>
+        <v>0.967741935483871</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8381877022653722</v>
+        <v>0.8419354838709677</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Logistic Regression Max R</t>
+          <t>Logistic Regression Multi-Max R</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9741100323624595</v>
+        <v>0.9709677419354839</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7702265372168284</v>
+        <v>0.7645161290322581</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Voting Classifier Max R</t>
+          <t>Voting Classifier Multi-Max R</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9676375404530745</v>
+        <v>0.967741935483871</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8284789644012945</v>
+        <v>0.8290322580645161</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Stacking Classifier Max R</t>
+          <t>Stacking Classifier Multi-Max R</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9644012944983819</v>
+        <v>0.964516129032258</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8058252427184466</v>
+        <v>0.8225806451612904</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update old model and add confusion, overall stats
</commit_message>
<xml_diff>
--- a/old_models/accuracies/max_r_model_accuracies.xlsx
+++ b/old_models/accuracies/max_r_model_accuracies.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>